<commit_message>
initial intergating optimize model
</commit_message>
<xml_diff>
--- a/references/Nutrition.xlsx
+++ b/references/Nutrition.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CCB8EB-EEDB-4E2F-884B-AA3266D19143}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBF9AAC-E68C-4A66-AA52-374F40A13A77}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="131">
   <si>
     <t>Nutrient</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Nutrient-vi</t>
   </si>
   <si>
-    <t>Kcal</t>
-  </si>
-  <si>
     <t>KJ</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>phytosterol</t>
+  </si>
+  <si>
+    <t>Cal</t>
   </si>
 </sst>
 </file>
@@ -527,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -536,23 +536,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -837,7 +833,7 @@
   <dimension ref="A1:AR41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -864,137 +860,137 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="R1" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="S1" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="V1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="W1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="X1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Y1" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Z1" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AA1" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AB1" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AC1" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AD1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AE1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AF1" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AG1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AH1" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AI1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AK1" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AL1" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AM1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AN1" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AO1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AP1" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AQ1" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AR1" s="8" t="s">
         <v>129</v>
-      </c>
-      <c r="AR1" s="11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:44">
@@ -1002,10 +998,10 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" t="s">
         <v>74</v>
-      </c>
-      <c r="G2" t="s">
-        <v>75</v>
       </c>
       <c r="H2" t="s">
         <v>2</v>
@@ -1121,16 +1117,16 @@
     </row>
     <row r="3" spans="1:44">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
         <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>78</v>
       </c>
       <c r="E3">
         <v>100</v>
@@ -1255,16 +1251,16 @@
     </row>
     <row r="4" spans="1:44">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
         <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" t="s">
-        <v>80</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -1389,16 +1385,16 @@
     </row>
     <row r="5" spans="1:44">
       <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
         <v>82</v>
       </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -1548,10 +1544,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1559,10 +1555,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1575,10 +1571,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1591,10 +1587,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1607,10 +1603,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1623,10 +1619,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1639,10 +1635,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1655,10 +1651,10 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1671,10 +1667,10 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1687,10 +1683,10 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1703,10 +1699,10 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1719,10 +1715,10 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1735,10 +1731,10 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1751,10 +1747,10 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1767,10 +1763,10 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1783,10 +1779,10 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1799,10 +1795,10 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1815,160 +1811,160 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="23.25">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="10"/>
+      <c r="B38" s="9"/>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B44" s="7" t="s">
+      <c r="A44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:2">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:2">
-      <c r="A49" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="5" t="s">
+      <c r="A49" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:2">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: init food controller and helper
</commit_message>
<xml_diff>
--- a/references/Nutrition.xlsx
+++ b/references/Nutrition.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20C8467-2DE6-47D2-8FAE-D6649D127775}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABBDAE-AD25-41CF-B963-7C569EB26B3C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="1605" windowWidth="17925" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -830,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR41"/>
+  <dimension ref="A1:AR5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AM4" sqref="AM4"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -846,7 +846,8 @@
     <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10.5703125" customWidth="1"/>
@@ -856,7 +857,9 @@
     <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
@@ -1517,10 +1520,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:44" ht="16.5" customHeight="1"/>
-    <row r="8" spans="1:44" ht="16.5" customHeight="1"/>
-    <row r="30" ht="21" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>